<commit_message>
chore: remove unwanted file
</commit_message>
<xml_diff>
--- a/public/static/reports/500097175_daily_report.xlsx
+++ b/public/static/reports/500097175_daily_report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quods\Documents\UPES\Interships\People_R(Social)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\adamalrahman\.code\web\e-portfolio\public\static\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733F7A6C-4096-430A-B0B3-1623B684A0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DEE4AE-70C4-409B-B23A-921F71C4EBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="117">
   <si>
     <t>Name of the NGO</t>
   </si>
@@ -381,10 +381,67 @@
     <t>6th July</t>
   </si>
   <si>
-    <t>7th - 30th July</t>
+    <t xml:space="preserve">    Because the organisation was busy we weren't assigned any work</t>
   </si>
   <si>
-    <t xml:space="preserve">    Because the organisation was busy we weren't assigned any work</t>
+    <t>no new work was assigned</t>
+  </si>
+  <si>
+    <t>The team had a discussion with Imthiyaz Sir.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We were given photos to edit. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team edited photos sent. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submitted a report assigned to write. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We had to draft and write a report. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edited more photos. </t>
+  </si>
+  <si>
+    <t>Editing of photos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submitted the photos. </t>
+  </si>
+  <si>
+    <t>7th July</t>
+  </si>
+  <si>
+    <t>8th July</t>
+  </si>
+  <si>
+    <t>9th July</t>
+  </si>
+  <si>
+    <t>10th July</t>
+  </si>
+  <si>
+    <t>11th - 31st July</t>
+  </si>
+  <si>
+    <t>Attended seminar held by Goonj Organisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning about Disaster Management, and the NGO's role during a crisis. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to use a fire extinguisher. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning a lot of new life skills. </t>
+  </si>
+  <si>
+    <t>Submitted report of event attended</t>
+  </si>
+  <si>
+    <t>weekend off</t>
   </si>
 </sst>
 </file>
@@ -394,7 +451,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +502,19 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -546,7 +616,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -563,6 +633,12 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -599,6 +675,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1807"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="79" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43:P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -893,7 +989,7 @@
     <col min="3" max="4" width="18" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="21.54296875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="16.54296875" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" style="7" customWidth="1"/>
     <col min="8" max="8" width="41.1796875" customWidth="1"/>
     <col min="9" max="9" width="95.36328125" customWidth="1"/>
     <col min="10" max="10" width="85.08984375" customWidth="1"/>
@@ -1110,17 +1206,17 @@
       <c r="G7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="18"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="20"/>
     </row>
     <row r="8" spans="1:16" s="1" customFormat="1">
       <c r="A8" s="11">
@@ -1138,17 +1234,17 @@
       <c r="G8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="21"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="11">
@@ -1366,17 +1462,17 @@
       <c r="G15" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="24"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="26"/>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="11">
@@ -1520,7 +1616,9 @@
       <c r="G19" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="12"/>
+      <c r="H19" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
@@ -1546,7 +1644,9 @@
       <c r="G20" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H20" s="12"/>
+      <c r="H20" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
@@ -1572,7 +1672,9 @@
       <c r="G21" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="3"/>
+      <c r="H21" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1598,19 +1700,19 @@
       <c r="G22" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="24"/>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="26"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.5">
       <c r="A23" s="11">
         <v>500097175</v>
       </c>
@@ -1626,8 +1728,12 @@
       <c r="G23" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="H23" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>99</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -1652,7 +1758,9 @@
       <c r="G24" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="3"/>
+      <c r="H24" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1678,7 +1786,9 @@
       <c r="G25" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1704,7 +1814,9 @@
       <c r="G26" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H26" s="3"/>
+      <c r="H26" s="32" t="s">
+        <v>100</v>
+      </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -1730,8 +1842,12 @@
       <c r="G27" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="H27" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>102</v>
+      </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -1756,8 +1872,12 @@
       <c r="G28" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="H28" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="I28" s="36" t="s">
+        <v>104</v>
+      </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -1782,17 +1902,17 @@
       <c r="G29" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H29" s="22" t="s">
+      <c r="H29" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="24"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="25"/>
+      <c r="P29" s="26"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="11">
@@ -1810,7 +1930,9 @@
       <c r="G30" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="H30" s="3"/>
+      <c r="H30" s="37" t="s">
+        <v>103</v>
+      </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1836,7 +1958,9 @@
       <c r="G31" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="H31" s="3"/>
+      <c r="H31" s="37" t="s">
+        <v>105</v>
+      </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -1862,7 +1986,9 @@
       <c r="G32" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="H32" s="3"/>
+      <c r="H32" s="37" t="s">
+        <v>97</v>
+      </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -1888,7 +2014,9 @@
       <c r="G33" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="H33" s="3"/>
+      <c r="H33" s="37" t="s">
+        <v>97</v>
+      </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -1914,7 +2042,9 @@
       <c r="G34" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H34" s="3"/>
+      <c r="H34" s="37" t="s">
+        <v>97</v>
+      </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -1940,7 +2070,9 @@
       <c r="G35" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H35" s="3"/>
+      <c r="H35" s="37" t="s">
+        <v>97</v>
+      </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -1966,17 +2098,17 @@
       <c r="G36" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H36" s="22" t="s">
+      <c r="H36" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="24"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="26"/>
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="11">
@@ -1994,7 +2126,9 @@
       <c r="G37" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H37" s="3"/>
+      <c r="H37" s="41" t="s">
+        <v>97</v>
+      </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2020,13 +2154,23 @@
       <c r="G38" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
+      <c r="H38" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="I38" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="J38" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="K38" s="45" t="s">
+        <v>113</v>
+      </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
+      <c r="N38" s="40" t="s">
+        <v>114</v>
+      </c>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
     </row>
@@ -2046,7 +2190,9 @@
       <c r="G39" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H39" s="3"/>
+      <c r="H39" s="46" t="s">
+        <v>115</v>
+      </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -2070,29 +2216,39 @@
         <v>22</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
-      <c r="H40" s="25" t="s">
+      <c r="H40" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="I40" s="26"/>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
-      <c r="L40" s="26"/>
-      <c r="M40" s="26"/>
-      <c r="N40" s="26"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="27"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="17"/>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="8"/>
-      <c r="B41" s="3"/>
+      <c r="A41" s="38">
+        <v>500097175</v>
+      </c>
+      <c r="B41" s="39" t="s">
+        <v>65</v>
+      </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="3"/>
+      <c r="F41" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H41" s="47" t="s">
+        <v>97</v>
+      </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2103,58 +2259,88 @@
       <c r="P41" s="3"/>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" s="8"/>
-      <c r="B42" s="3"/>
+      <c r="A42" s="38">
+        <v>500097175</v>
+      </c>
+      <c r="B42" s="39" t="s">
+        <v>65</v>
+      </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
+      <c r="F42" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H42" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="26"/>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="8"/>
-      <c r="B43" s="3"/>
+      <c r="A43" s="38">
+        <v>500097175</v>
+      </c>
+      <c r="B43" s="39" t="s">
+        <v>65</v>
+      </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
+      <c r="F43" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H43" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+      <c r="O43" s="25"/>
+      <c r="P43" s="26"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="8"/>
-      <c r="B44" s="3"/>
+      <c r="A44" s="38">
+        <v>500097175</v>
+      </c>
+      <c r="B44" s="39" t="s">
+        <v>65</v>
+      </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
+      <c r="F44" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H44" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="28"/>
+      <c r="P44" s="29"/>
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="8"/>
@@ -33891,11 +34077,13 @@
       <c r="P1807" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="H44:P44"/>
+    <mergeCell ref="H42:P42"/>
+    <mergeCell ref="H43:P43"/>
     <mergeCell ref="H7:P7"/>
     <mergeCell ref="H8:P8"/>
     <mergeCell ref="H15:P15"/>
-    <mergeCell ref="H40:P40"/>
     <mergeCell ref="H22:P22"/>
     <mergeCell ref="H29:P29"/>
     <mergeCell ref="H36:P36"/>

</xml_diff>